<commit_message>
Added script for variance increasing type
</commit_message>
<xml_diff>
--- a/dna-methylation/scripts/develop/illumina450k/betas/plot/scatter_comparison_cols.xlsx
+++ b/dna-methylation/scripts/develop/illumina450k/betas/plot/scatter_comparison_cols.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\dna-methylation\dna-methylation\scripts\develop\illumina450k\betas\plot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dna-methylation\dna-methylation\scripts\develop\illumina450k\betas\plot\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DC0A7E-637A-4513-A578-6EA3706FF0B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="33120" windowHeight="18120"/>
+    <workbookView xWindow="13410" yWindow="3225" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="i" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>data_bases</t>
   </si>
@@ -33,13 +34,19 @@
     <t>GSE87571</t>
   </si>
   <si>
-    <t>E-MTAB-7309-FILTERED</t>
+    <t>GSE40279</t>
+  </si>
+  <si>
+    <t>EPIC</t>
+  </si>
+  <si>
+    <t>GSE55763</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -190,6 +197,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -225,6 +249,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -400,14 +441,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -439,6 +483,28 @@
         <v>5</v>
       </c>
       <c r="C3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
         <v>105</v>
       </c>
     </row>

</xml_diff>